<commit_message>
add lpat on database
</commit_message>
<xml_diff>
--- a/app/database/seeds/seed_files/masterfile2.xlsx
+++ b/app/database/seeds/seed_files/masterfile2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="activity_grouping" sheetId="11" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="users" sheetId="8" r:id="rId7"/>
     <sheet name="objective" sheetId="9" r:id="rId8"/>
     <sheet name="source" sheetId="10" r:id="rId9"/>
+    <sheet name="scope" sheetId="12" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">sku!$A$1:$L$835</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4211" uniqueCount="1915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4216" uniqueCount="1920">
   <si>
     <t>activity_type_code</t>
   </si>
@@ -5771,6 +5772,21 @@
   </si>
   <si>
     <t>STICKERING</t>
+  </si>
+  <si>
+    <t>objective_id</t>
+  </si>
+  <si>
+    <t>scope_id</t>
+  </si>
+  <si>
+    <t>CUSTOMIZED</t>
+  </si>
+  <si>
+    <t>NATIONAL</t>
+  </si>
+  <si>
+    <t>scope</t>
   </si>
 </sst>
 </file>
@@ -6233,11 +6249,53 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -43733,62 +43791,94 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B1" t="s">
         <v>1904</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>1890</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>1891</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>1892</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>1893</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>1894</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>1895</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>1896</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>1897</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>1898</v>
       </c>
     </row>

</xml_diff>